<commit_message>
add reporting node parents
</commit_message>
<xml_diff>
--- a/PresentValueSeries/Dimensions.xlsx
+++ b/PresentValueSeries/Dimensions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4817EA-A71E-4899-AD69-2EB287A69F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0D36A3-DFA7-4AF8-AEF0-BBE73E39CA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14133" tabRatio="874" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9947" yWindow="887" windowWidth="12946" windowHeight="10393" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingNode" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="321">
   <si>
     <t>SystemName</t>
   </si>
@@ -1136,16 +1136,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2915,8 +2913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC69F85-C9AE-4FC5-8D78-4F30166B2B3D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2959,6 +2957,9 @@
       <c r="B3" t="s">
         <v>312</v>
       </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -2969,6 +2970,9 @@
       </c>
       <c r="B4" t="s">
         <v>311</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -3556,17 +3560,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
         <v>318</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>319</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>224</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>27</v>
       </c>
     </row>
@@ -3598,17 +3602,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
         <v>320</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" t="s">
         <v>319</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32">
         <v>30</v>
       </c>
     </row>
@@ -3634,28 +3638,28 @@
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6">
         <v>10</v>
       </c>
     </row>
@@ -4306,28 +4310,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
         <v>308</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>309</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
         <v>307</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>310</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>308</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>40</v>
       </c>
     </row>
@@ -5393,7 +5397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90D6FDA-5CB2-4E6F-BD5A-98362BAFEEDE}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -6264,41 +6268,41 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A4">
         <v>1900</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>307</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>232</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>289</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4">
         <v>30</v>
       </c>
     </row>
@@ -7064,13 +7068,13 @@
       <c r="B2" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>135</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>44</v>
       </c>
       <c r="F2">
@@ -7084,36 +7088,36 @@
       <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>44</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>315</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>15</v>
       </c>
     </row>
@@ -7124,13 +7128,13 @@
       <c r="B5" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>291</v>
       </c>
       <c r="F5">
@@ -7144,13 +7148,13 @@
       <c r="B6" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>135</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>291</v>
       </c>
       <c r="F6">
@@ -7164,13 +7168,13 @@
       <c r="B7" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>291</v>
       </c>
       <c r="F7">
@@ -7184,13 +7188,13 @@
       <c r="B8" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>291</v>
       </c>
       <c r="F8">
@@ -7204,13 +7208,13 @@
       <c r="B9" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>291</v>
       </c>
       <c r="F9">
@@ -7233,13 +7237,13 @@
       <c r="B10" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>291</v>
       </c>
       <c r="F10">
@@ -7262,13 +7266,13 @@
       <c r="B11" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
         <v>135</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>291</v>
       </c>
       <c r="F11">
@@ -7282,13 +7286,13 @@
       <c r="B12" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
         <v>145</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>291</v>
       </c>
       <c r="F12">
@@ -7302,13 +7306,13 @@
       <c r="B13" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>291</v>
       </c>
       <c r="F13">
@@ -7322,13 +7326,13 @@
       <c r="B14" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>291</v>
       </c>
       <c r="F14">
@@ -7342,13 +7346,13 @@
       <c r="B15" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>291</v>
       </c>
       <c r="F15">
@@ -7362,13 +7366,13 @@
       <c r="B16" t="s">
         <v>153</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
         <v>145</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>291</v>
       </c>
       <c r="F16">
@@ -7382,13 +7386,13 @@
       <c r="B17" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
         <v>145</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>291</v>
       </c>
       <c r="F17">

</xml_diff>

<commit_message>
Improving present value documentation (#164)
* add reporting node parents

* picture

* better documentation

Co-authored-by: Andrea Muolo <amuolo@systemorph.com>
</commit_message>
<xml_diff>
--- a/PresentValueSeries/Dimensions.xlsx
+++ b/PresentValueSeries/Dimensions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4817EA-A71E-4899-AD69-2EB287A69F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3141EF-BB0B-48EC-89BF-984367045A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14133" tabRatio="874" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14133" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingNode" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="321">
   <si>
     <t>SystemName</t>
   </si>
@@ -1136,16 +1136,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2915,8 +2913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC69F85-C9AE-4FC5-8D78-4F30166B2B3D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2959,6 +2957,9 @@
       <c r="B3" t="s">
         <v>312</v>
       </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -2969,6 +2970,9 @@
       </c>
       <c r="B4" t="s">
         <v>311</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -3556,17 +3560,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
         <v>318</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>319</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>224</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>27</v>
       </c>
     </row>
@@ -3598,17 +3602,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
         <v>320</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" t="s">
         <v>319</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32">
         <v>30</v>
       </c>
     </row>
@@ -3634,28 +3638,28 @@
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6">
         <v>10</v>
       </c>
     </row>
@@ -4306,28 +4310,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
         <v>308</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>309</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
         <v>307</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>310</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>308</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>40</v>
       </c>
     </row>
@@ -5393,8 +5397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90D6FDA-5CB2-4E6F-BD5A-98362BAFEEDE}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -6264,41 +6268,41 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A4">
         <v>1900</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>307</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>232</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>289</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4">
         <v>30</v>
       </c>
     </row>
@@ -7064,13 +7068,13 @@
       <c r="B2" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>135</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>44</v>
       </c>
       <c r="F2">
@@ -7084,36 +7088,36 @@
       <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>44</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>315</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>15</v>
       </c>
     </row>
@@ -7124,13 +7128,13 @@
       <c r="B5" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>291</v>
       </c>
       <c r="F5">
@@ -7144,13 +7148,13 @@
       <c r="B6" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>135</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>291</v>
       </c>
       <c r="F6">
@@ -7164,13 +7168,13 @@
       <c r="B7" t="s">
         <v>142</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>291</v>
       </c>
       <c r="F7">
@@ -7184,13 +7188,13 @@
       <c r="B8" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>291</v>
       </c>
       <c r="F8">
@@ -7204,13 +7208,13 @@
       <c r="B9" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>291</v>
       </c>
       <c r="F9">
@@ -7233,13 +7237,13 @@
       <c r="B10" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>291</v>
       </c>
       <c r="F10">
@@ -7262,13 +7266,13 @@
       <c r="B11" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
         <v>135</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>291</v>
       </c>
       <c r="F11">
@@ -7282,13 +7286,13 @@
       <c r="B12" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
         <v>145</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>291</v>
       </c>
       <c r="F12">
@@ -7302,13 +7306,13 @@
       <c r="B13" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>291</v>
       </c>
       <c r="F13">
@@ -7322,13 +7326,13 @@
       <c r="B14" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>291</v>
       </c>
       <c r="F14">
@@ -7342,13 +7346,13 @@
       <c r="B15" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>291</v>
       </c>
       <c r="F15">
@@ -7362,13 +7366,13 @@
       <c r="B16" t="s">
         <v>153</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
         <v>145</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>291</v>
       </c>
       <c r="F16">
@@ -7382,13 +7386,13 @@
       <c r="B17" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>4</v>
       </c>
       <c r="D17" t="s">
         <v>145</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>291</v>
       </c>
       <c r="F17">

</xml_diff>

<commit_message>
remove parent from RN in Dimensions.xlsx
</commit_message>
<xml_diff>
--- a/PresentValueSeries/Dimensions.xlsx
+++ b/PresentValueSeries/Dimensions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3141EF-BB0B-48EC-89BF-984367045A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AD66A1-1437-4D02-B122-278FBEF186B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14133" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingNode" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="321">
   <si>
     <t>SystemName</t>
   </si>
@@ -2903,7 +2903,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2914,10 +2914,10 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -2925,7 +2925,7 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2950,29 +2950,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>312</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>306</v>
       </c>
       <c r="B4" t="s">
         <v>311</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -3003,13 +2997,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3017,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -3025,7 +3019,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3033,7 +3027,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -3058,13 +3052,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3072,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -3080,7 +3074,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3088,7 +3082,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -3096,7 +3090,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3104,7 +3098,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3112,7 +3106,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -3120,7 +3114,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -3128,7 +3122,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -3136,7 +3130,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -3163,7 +3157,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
@@ -3171,7 +3165,7 @@
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3185,7 +3179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -3196,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -3210,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -3224,7 +3218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -3238,7 +3232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>187</v>
       </c>
@@ -3252,7 +3246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -3266,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>190</v>
       </c>
@@ -3280,7 +3274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -3294,7 +3288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>194</v>
       </c>
@@ -3308,7 +3302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>196</v>
       </c>
@@ -3322,7 +3316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>198</v>
       </c>
@@ -3336,7 +3330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>200</v>
       </c>
@@ -3350,7 +3344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
@@ -3364,7 +3358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>204</v>
       </c>
@@ -3378,7 +3372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>205</v>
       </c>
@@ -3392,7 +3386,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>207</v>
       </c>
@@ -3406,7 +3400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>209</v>
       </c>
@@ -3420,7 +3414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>210</v>
       </c>
@@ -3434,7 +3428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>212</v>
       </c>
@@ -3448,7 +3442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>214</v>
       </c>
@@ -3462,7 +3456,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>216</v>
       </c>
@@ -3476,7 +3470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>218</v>
       </c>
@@ -3490,7 +3484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>220</v>
       </c>
@@ -3504,7 +3498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>222</v>
       </c>
@@ -3518,7 +3512,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>224</v>
       </c>
@@ -3532,7 +3526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>226</v>
       </c>
@@ -3546,7 +3540,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -3560,7 +3554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>318</v>
       </c>
@@ -3574,7 +3568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>230</v>
       </c>
@@ -3588,7 +3582,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>231</v>
       </c>
@@ -3602,7 +3596,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>320</v>
       </c>
@@ -3635,9 +3629,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3651,7 +3645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>316</v>
       </c>
@@ -3674,14 +3668,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3692,7 +3686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>232</v>
       </c>
@@ -3703,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -3714,7 +3708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -3742,13 +3736,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3756,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -3764,7 +3758,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -3772,7 +3766,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -3799,13 +3793,13 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3813,7 +3807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -3838,13 +3832,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3852,7 +3846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -3877,7 +3871,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -3885,7 +3879,7 @@
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3899,7 +3893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -3934,7 +3928,7 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
@@ -3942,7 +3936,7 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3956,7 +3950,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>238</v>
       </c>
@@ -3970,7 +3964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3984,7 +3978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>242</v>
       </c>
@@ -3998,7 +3992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -4012,7 +4006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>246</v>
       </c>
@@ -4026,7 +4020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>248</v>
       </c>
@@ -4040,7 +4034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4054,7 +4048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4068,7 +4062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>254</v>
       </c>
@@ -4082,7 +4076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>256</v>
       </c>
@@ -4096,7 +4090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>258</v>
       </c>
@@ -4110,7 +4104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>260</v>
       </c>
@@ -4124,7 +4118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>262</v>
       </c>
@@ -4138,7 +4132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>264</v>
       </c>
@@ -4152,7 +4146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>266</v>
       </c>
@@ -4166,7 +4160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>268</v>
       </c>
@@ -4180,7 +4174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>270</v>
       </c>
@@ -4194,7 +4188,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>272</v>
       </c>
@@ -4208,7 +4202,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>274</v>
       </c>
@@ -4222,7 +4216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>276</v>
       </c>
@@ -4255,15 +4249,15 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4277,7 +4271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4288,7 +4282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4299,7 +4293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>313</v>
       </c>
@@ -4310,7 +4304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>308</v>
       </c>
@@ -4321,7 +4315,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>307</v>
       </c>
@@ -4335,7 +4329,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -4346,7 +4340,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -4357,7 +4351,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -4368,7 +4362,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4379,7 +4373,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4393,7 +4387,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -4407,7 +4401,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -4418,7 +4412,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -4429,7 +4423,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -4440,7 +4434,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -4451,7 +4445,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -4462,7 +4456,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -4473,7 +4467,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -4506,7 +4500,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
@@ -4515,7 +4509,7 @@
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4532,7 +4526,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -4549,7 +4543,7 @@
         <v>1.2012</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4566,7 +4560,7 @@
         <v>1.2013</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -4583,7 +4577,7 @@
         <v>1.2014</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4600,7 +4594,7 @@
         <v>1.2015</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -4617,7 +4611,7 @@
         <v>1.2016</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -4634,7 +4628,7 @@
         <v>1.2017</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -4651,7 +4645,7 @@
         <v>1.2018</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -4668,7 +4662,7 @@
         <v>1.2019</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4685,7 +4679,7 @@
         <v>1.4016</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4702,7 +4696,7 @@
         <v>1.4016999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -4719,7 +4713,7 @@
         <v>1.4017999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4761,7 +4755,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
@@ -4770,7 +4764,7 @@
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>278</v>
       </c>
@@ -4790,7 +4784,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -4810,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -4830,7 +4824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -4844,7 +4838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -4858,7 +4852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -4869,7 +4863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -4877,7 +4871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -4885,7 +4879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -4893,7 +4887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -4901,7 +4895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -4909,7 +4903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -4917,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -4925,457 +4919,457 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1982</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1983</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1984</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1985</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1986</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1987</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1988</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1989</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1990</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1991</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1992</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1993</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1994</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1995</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1996</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1997</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1998</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1999</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2001</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2002</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2003</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2004</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2005</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2006</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2007</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2008</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2009</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2010</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2012</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2014</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2015</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2016</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2017</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2018</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2019</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2020</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2021</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2022</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2023</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2024</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2025</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2026</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2027</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2028</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2029</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2030</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2031</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2032</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2033</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2034</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2035</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2036</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2037</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2038</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2039</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2040</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2041</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2042</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2043</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2044</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2045</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2046</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2047</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2048</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2049</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2050</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2051</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2052</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2053</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2054</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2055</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2056</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2057</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2058</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2059</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2060</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2061</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2062</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2063</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2064</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2065</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2066</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2067</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2068</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2069</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2070</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2071</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2072</v>
       </c>
@@ -5401,7 +5395,7 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
@@ -5411,7 +5405,7 @@
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5431,7 +5425,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5445,7 +5439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -5486,7 +5480,7 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
@@ -5497,7 +5491,7 @@
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5520,7 +5514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -5540,7 +5534,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5554,7 +5548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -5577,7 +5571,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -5600,7 +5594,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -5617,7 +5611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -5634,7 +5628,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -5651,7 +5645,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -5668,7 +5662,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -5682,7 +5676,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -5699,7 +5693,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -5716,7 +5710,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -5730,7 +5724,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -5744,7 +5738,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -5761,7 +5755,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -5802,13 +5796,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5833,14 +5827,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5851,7 +5845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -5859,7 +5853,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -5889,7 +5883,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
@@ -5897,7 +5891,7 @@
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5911,7 +5905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -5922,7 +5916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -5936,7 +5930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -5950,7 +5944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -5964,7 +5958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -5978,7 +5972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -5992,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -6006,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -6020,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -6034,7 +6028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -6048,7 +6042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -6062,7 +6056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -6076,7 +6070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>122</v>
       </c>
@@ -6090,7 +6084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -6104,7 +6098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>126</v>
       </c>
@@ -6142,11 +6136,11 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.8203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.17578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
@@ -6154,7 +6148,7 @@
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>278</v>
       </c>
@@ -6192,7 +6186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1900</v>
       </c>
@@ -6230,7 +6224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1900</v>
       </c>
@@ -6268,7 +6262,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1900</v>
       </c>
@@ -6306,7 +6300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1900</v>
       </c>
@@ -6344,7 +6338,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1900</v>
       </c>
@@ -6382,7 +6376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1900</v>
       </c>
@@ -6420,7 +6414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1900</v>
       </c>
@@ -6458,7 +6452,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1900</v>
       </c>
@@ -6496,7 +6490,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1900</v>
       </c>
@@ -6534,7 +6528,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1900</v>
       </c>
@@ -6572,7 +6566,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1900</v>
       </c>
@@ -6610,7 +6604,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1900</v>
       </c>
@@ -6648,7 +6642,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1900</v>
       </c>
@@ -6686,7 +6680,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1900</v>
       </c>
@@ -6724,7 +6718,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1900</v>
       </c>
@@ -6762,7 +6756,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1900</v>
       </c>
@@ -6800,7 +6794,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1900</v>
       </c>
@@ -6838,7 +6832,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1900</v>
       </c>
@@ -6876,7 +6870,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1900</v>
       </c>
@@ -6914,7 +6908,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1900</v>
       </c>
@@ -6952,7 +6946,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1900</v>
       </c>
@@ -7020,7 +7014,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
@@ -7032,7 +7026,7 @@
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7061,7 +7055,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -7081,7 +7075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -7101,7 +7095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -7121,7 +7115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -7141,7 +7135,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -7161,7 +7155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -7181,7 +7175,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>143</v>
       </c>
@@ -7201,7 +7195,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -7230,7 +7224,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>148</v>
       </c>
@@ -7259,7 +7253,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>150</v>
       </c>
@@ -7279,7 +7273,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -7299,7 +7293,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -7319,7 +7313,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>157</v>
       </c>
@@ -7339,7 +7333,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>158</v>
       </c>
@@ -7359,7 +7353,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>159</v>
       </c>
@@ -7379,7 +7373,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
Fix pv ep2 (#207)
remove parent from RN in Dimensions.xlsx
</commit_message>
<xml_diff>
--- a/PresentValueSeries/Dimensions.xlsx
+++ b/PresentValueSeries/Dimensions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3141EF-BB0B-48EC-89BF-984367045A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AD66A1-1437-4D02-B122-278FBEF186B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14133" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingNode" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="321">
   <si>
     <t>SystemName</t>
   </si>
@@ -2903,7 +2903,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2914,10 +2914,10 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -2925,7 +2925,7 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2950,29 +2950,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>312</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>306</v>
       </c>
       <c r="B4" t="s">
         <v>311</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -3003,13 +2997,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3017,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -3025,7 +3019,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3033,7 +3027,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -3058,13 +3052,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3072,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -3080,7 +3074,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3088,7 +3082,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -3096,7 +3090,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3104,7 +3098,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3112,7 +3106,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -3120,7 +3114,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -3128,7 +3122,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -3136,7 +3130,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>178</v>
       </c>
@@ -3163,7 +3157,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
@@ -3171,7 +3165,7 @@
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3185,7 +3179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -3196,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -3210,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -3224,7 +3218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -3238,7 +3232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>187</v>
       </c>
@@ -3252,7 +3246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -3266,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>190</v>
       </c>
@@ -3280,7 +3274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -3294,7 +3288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>194</v>
       </c>
@@ -3308,7 +3302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>196</v>
       </c>
@@ -3322,7 +3316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>198</v>
       </c>
@@ -3336,7 +3330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>200</v>
       </c>
@@ -3350,7 +3344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
@@ -3364,7 +3358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>204</v>
       </c>
@@ -3378,7 +3372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>205</v>
       </c>
@@ -3392,7 +3386,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>207</v>
       </c>
@@ -3406,7 +3400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>209</v>
       </c>
@@ -3420,7 +3414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>210</v>
       </c>
@@ -3434,7 +3428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>212</v>
       </c>
@@ -3448,7 +3442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>214</v>
       </c>
@@ -3462,7 +3456,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>216</v>
       </c>
@@ -3476,7 +3470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>218</v>
       </c>
@@ -3490,7 +3484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>220</v>
       </c>
@@ -3504,7 +3498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>222</v>
       </c>
@@ -3518,7 +3512,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>224</v>
       </c>
@@ -3532,7 +3526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>226</v>
       </c>
@@ -3546,7 +3540,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -3560,7 +3554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>318</v>
       </c>
@@ -3574,7 +3568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>230</v>
       </c>
@@ -3588,7 +3582,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>231</v>
       </c>
@@ -3602,7 +3596,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>320</v>
       </c>
@@ -3635,9 +3629,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3651,7 +3645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>316</v>
       </c>
@@ -3674,14 +3668,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3692,7 +3686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>232</v>
       </c>
@@ -3703,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -3714,7 +3708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -3742,13 +3736,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3756,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -3764,7 +3758,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -3772,7 +3766,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -3799,13 +3793,13 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3813,7 +3807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -3838,13 +3832,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3852,7 +3846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -3877,7 +3871,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -3885,7 +3879,7 @@
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3899,7 +3893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -3934,7 +3928,7 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
@@ -3942,7 +3936,7 @@
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3956,7 +3950,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>238</v>
       </c>
@@ -3970,7 +3964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3984,7 +3978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>242</v>
       </c>
@@ -3998,7 +3992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -4012,7 +4006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>246</v>
       </c>
@@ -4026,7 +4020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>248</v>
       </c>
@@ -4040,7 +4034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -4054,7 +4048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -4068,7 +4062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>254</v>
       </c>
@@ -4082,7 +4076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>256</v>
       </c>
@@ -4096,7 +4090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>258</v>
       </c>
@@ -4110,7 +4104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>260</v>
       </c>
@@ -4124,7 +4118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>262</v>
       </c>
@@ -4138,7 +4132,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>264</v>
       </c>
@@ -4152,7 +4146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>266</v>
       </c>
@@ -4166,7 +4160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>268</v>
       </c>
@@ -4180,7 +4174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>270</v>
       </c>
@@ -4194,7 +4188,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>272</v>
       </c>
@@ -4208,7 +4202,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>274</v>
       </c>
@@ -4222,7 +4216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>276</v>
       </c>
@@ -4255,15 +4249,15 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4277,7 +4271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4288,7 +4282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4299,7 +4293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>313</v>
       </c>
@@ -4310,7 +4304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>308</v>
       </c>
@@ -4321,7 +4315,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>307</v>
       </c>
@@ -4335,7 +4329,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -4346,7 +4340,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -4357,7 +4351,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -4368,7 +4362,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -4379,7 +4373,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4393,7 +4387,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -4407,7 +4401,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -4418,7 +4412,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -4429,7 +4423,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -4440,7 +4434,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -4451,7 +4445,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -4462,7 +4456,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -4473,7 +4467,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -4506,7 +4500,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
@@ -4515,7 +4509,7 @@
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4532,7 +4526,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -4549,7 +4543,7 @@
         <v>1.2012</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -4566,7 +4560,7 @@
         <v>1.2013</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -4583,7 +4577,7 @@
         <v>1.2014</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4600,7 +4594,7 @@
         <v>1.2015</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -4617,7 +4611,7 @@
         <v>1.2016</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -4634,7 +4628,7 @@
         <v>1.2017</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -4651,7 +4645,7 @@
         <v>1.2018</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -4668,7 +4662,7 @@
         <v>1.2019</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4685,7 +4679,7 @@
         <v>1.4016</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4702,7 +4696,7 @@
         <v>1.4016999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -4719,7 +4713,7 @@
         <v>1.4017999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4761,7 +4755,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
@@ -4770,7 +4764,7 @@
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>278</v>
       </c>
@@ -4790,7 +4784,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1970</v>
       </c>
@@ -4810,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -4830,7 +4824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1972</v>
       </c>
@@ -4844,7 +4838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1973</v>
       </c>
@@ -4858,7 +4852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1974</v>
       </c>
@@ -4869,7 +4863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1975</v>
       </c>
@@ -4877,7 +4871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1976</v>
       </c>
@@ -4885,7 +4879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1977</v>
       </c>
@@ -4893,7 +4887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1978</v>
       </c>
@@ -4901,7 +4895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1979</v>
       </c>
@@ -4909,7 +4903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1980</v>
       </c>
@@ -4917,7 +4911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1981</v>
       </c>
@@ -4925,457 +4919,457 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1982</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1983</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1984</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1985</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1986</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1987</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1988</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1989</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1990</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1991</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1992</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1993</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1994</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1995</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1996</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1997</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1998</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1999</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2001</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2002</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2003</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2004</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2005</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2006</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2007</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2008</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2009</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2010</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2011</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2012</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2014</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2015</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2016</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2017</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2018</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2019</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2020</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2021</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2022</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2023</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2024</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2025</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2026</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2027</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2028</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2029</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2030</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2031</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2032</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2033</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2034</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2035</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2036</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2037</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2038</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2039</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2040</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2041</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2042</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2043</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2044</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2045</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2046</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2047</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2048</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2049</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2050</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2051</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2052</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2053</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2054</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2055</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2056</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2057</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2058</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2059</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2060</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2061</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2062</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2063</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2064</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2065</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2066</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2067</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2068</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2069</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2070</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2071</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2072</v>
       </c>
@@ -5401,7 +5395,7 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
@@ -5411,7 +5405,7 @@
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5431,7 +5425,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5445,7 +5439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -5486,7 +5480,7 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
@@ -5497,7 +5491,7 @@
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5520,7 +5514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -5540,7 +5534,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5554,7 +5548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -5577,7 +5571,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -5600,7 +5594,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -5617,7 +5611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -5634,7 +5628,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -5651,7 +5645,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -5668,7 +5662,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -5682,7 +5676,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -5699,7 +5693,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -5716,7 +5710,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -5730,7 +5724,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -5744,7 +5738,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -5761,7 +5755,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -5802,13 +5796,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5833,14 +5827,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5851,7 +5845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -5859,7 +5853,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -5889,7 +5883,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
@@ -5897,7 +5891,7 @@
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5911,7 +5905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -5922,7 +5916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -5936,7 +5930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -5950,7 +5944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -5964,7 +5958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -5978,7 +5972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -5992,7 +5986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -6006,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -6020,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -6034,7 +6028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -6048,7 +6042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -6062,7 +6056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -6076,7 +6070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>122</v>
       </c>
@@ -6090,7 +6084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -6104,7 +6098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>126</v>
       </c>
@@ -6142,11 +6136,11 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.8203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.17578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
@@ -6154,7 +6148,7 @@
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>278</v>
       </c>
@@ -6192,7 +6186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1900</v>
       </c>
@@ -6230,7 +6224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1900</v>
       </c>
@@ -6268,7 +6262,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1900</v>
       </c>
@@ -6306,7 +6300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1900</v>
       </c>
@@ -6344,7 +6338,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1900</v>
       </c>
@@ -6382,7 +6376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1900</v>
       </c>
@@ -6420,7 +6414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1900</v>
       </c>
@@ -6458,7 +6452,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1900</v>
       </c>
@@ -6496,7 +6490,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1900</v>
       </c>
@@ -6534,7 +6528,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1900</v>
       </c>
@@ -6572,7 +6566,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1900</v>
       </c>
@@ -6610,7 +6604,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1900</v>
       </c>
@@ -6648,7 +6642,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1900</v>
       </c>
@@ -6686,7 +6680,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1900</v>
       </c>
@@ -6724,7 +6718,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1900</v>
       </c>
@@ -6762,7 +6756,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1900</v>
       </c>
@@ -6800,7 +6794,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1900</v>
       </c>
@@ -6838,7 +6832,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1900</v>
       </c>
@@ -6876,7 +6870,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1900</v>
       </c>
@@ -6914,7 +6908,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1900</v>
       </c>
@@ -6952,7 +6946,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1900</v>
       </c>
@@ -7020,7 +7014,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
@@ -7032,7 +7026,7 @@
     <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7061,7 +7055,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -7081,7 +7075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -7101,7 +7095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -7121,7 +7115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -7141,7 +7135,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -7161,7 +7155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -7181,7 +7175,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>143</v>
       </c>
@@ -7201,7 +7195,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -7230,7 +7224,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>148</v>
       </c>
@@ -7259,7 +7253,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>150</v>
       </c>
@@ -7279,7 +7273,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -7299,7 +7293,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -7319,7 +7313,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>157</v>
       </c>
@@ -7339,7 +7333,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>158</v>
       </c>
@@ -7359,7 +7353,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>159</v>
       </c>
@@ -7379,7 +7373,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>160</v>
       </c>

</xml_diff>